<commit_message>
loads county level crop production data for calculation of county level outputs
</commit_message>
<xml_diff>
--- a/RawData/Pfeedsupplementprod.xlsx
+++ b/RawData/Pfeedsupplementprod.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malgren/Documents/Mines/N_P/NANI_NAPI/CSNAPNIv1/RawData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A44E2FBC-4839-A146-A992-88AA057131E6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD96DE7-6989-EE45-A1D6-C10040186C84}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23900" yWindow="-22120" windowWidth="26840" windowHeight="15940" xr2:uid="{B337FA75-AAC9-E84C-8A12-4A38C0F69304}"/>
+    <workbookView xWindow="-13280" yWindow="-23760" windowWidth="26840" windowHeight="15940" xr2:uid="{B337FA75-AAC9-E84C-8A12-4A38C0F69304}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="USDA fertilizer conversion" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="79">
   <si>
     <t>US P mining</t>
   </si>
@@ -251,9 +252,6 @@
     <t>US P fertilizer exports (PFE)</t>
   </si>
   <si>
-    <t>CSNAPNI estimation</t>
-  </si>
-  <si>
     <t>Calculated: PAP = [PRM + PRI - PRE] * propPAP</t>
   </si>
   <si>
@@ -264,12 +262,27 @@
   </si>
   <si>
     <t>US P supplement availability (PSA)</t>
+  </si>
+  <si>
+    <t>USDA Fertilizer Use and Price tables (1997-2012), CSNAPNI estimation (2017)</t>
+  </si>
+  <si>
+    <t>1000 short tons P</t>
+  </si>
+  <si>
+    <t>kg/short ton</t>
+  </si>
+  <si>
+    <t>From Table 1, US consumption of plant nutrients</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="10">
     <font>
       <sz val="12"/>
@@ -459,7 +472,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -495,15 +508,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -524,6 +528,21 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -2047,7 +2066,7 @@
   <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="B15" sqref="B15:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2068,36 +2087,36 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" s="16"/>
-      <c r="B1" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="20"/>
+      <c r="B1" s="30" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="32"/>
+      <c r="G1" s="17"/>
       <c r="I1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="21"/>
-      <c r="B2" s="22">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19">
         <v>1997</v>
       </c>
-      <c r="C2" s="23">
+      <c r="C2" s="20">
         <v>2002</v>
       </c>
-      <c r="D2" s="23">
+      <c r="D2" s="20">
         <v>2007</v>
       </c>
-      <c r="E2" s="23">
+      <c r="E2" s="20">
         <v>2012</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="21">
         <v>2017</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="22" t="s">
         <v>15</v>
       </c>
       <c r="J2">
@@ -2120,27 +2139,27 @@
       <c r="A3" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="B3" s="26">
+      <c r="B3" s="23">
         <f>J3*10^6*J8/10^9</f>
         <v>6.0168221709006922</v>
       </c>
-      <c r="C3" s="27">
+      <c r="C3" s="24">
         <f>K3*10^6*K8/10^9</f>
         <v>4.601</v>
       </c>
-      <c r="D3" s="27">
+      <c r="D3" s="24">
         <f>L3*10^6*L8/10^9</f>
         <v>3.6463999999999999</v>
       </c>
-      <c r="E3" s="27">
+      <c r="E3" s="24">
         <f>M3*10^6*M8/10^9</f>
         <v>3.6936999999999993</v>
       </c>
-      <c r="F3" s="28">
+      <c r="F3" s="25">
         <f>N3*10^6*N8/10^9</f>
         <v>3.3109999999999995</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="G3" s="26" t="s">
         <v>24</v>
       </c>
       <c r="I3" t="s">
@@ -2166,27 +2185,27 @@
       <c r="A4" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B4" s="26">
+      <c r="B4" s="23">
         <f>J4*10^6*J8/10^9</f>
         <v>0.23988637413394917</v>
       </c>
-      <c r="C4" s="27">
+      <c r="C4" s="24">
         <f>K4*10^6*K8/10^9</f>
         <v>0.34411911357340724</v>
       </c>
-      <c r="D4" s="27">
+      <c r="D4" s="24">
         <f>L4*10^6*L8/10^9</f>
         <v>0.32780767676767675</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="24">
         <f>M4*10^6*M8/10^9</f>
         <v>0.43808999999999998</v>
       </c>
-      <c r="F4" s="28">
+      <c r="F4" s="25">
         <f>N4*10^6*N8/10^9</f>
         <v>0.29905806451612904</v>
       </c>
-      <c r="G4" s="29" t="s">
+      <c r="G4" s="26" t="s">
         <v>24</v>
       </c>
       <c r="I4" t="s">
@@ -2221,26 +2240,26 @@
       <c r="A5" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B5" s="26">
+      <c r="B5" s="23">
         <f>J5*10^6*J8/10^9</f>
         <v>4.3913625866050805E-2</v>
       </c>
-      <c r="C5" s="27">
+      <c r="C5" s="24">
         <f>K5*10^6*K8/10^9</f>
         <v>4.9706094182825492E-3</v>
       </c>
-      <c r="D5" s="27">
+      <c r="D5" s="24">
         <v>0</v>
       </c>
-      <c r="E5" s="27">
+      <c r="E5" s="24">
         <f>M5*10^6*M8/10^9</f>
         <v>0</v>
       </c>
-      <c r="F5" s="28">
+      <c r="F5" s="25">
         <f>N5*10^6*N8/10^9</f>
         <v>0</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="26" t="s">
         <v>24</v>
       </c>
       <c r="I5" t="s">
@@ -2266,22 +2285,22 @@
       <c r="A6" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="B6" s="26">
+      <c r="B6" s="23">
         <v>0.9</v>
       </c>
-      <c r="C6" s="27">
+      <c r="C6" s="24">
         <v>0.95</v>
       </c>
-      <c r="D6" s="27">
+      <c r="D6" s="24">
         <v>0.95</v>
       </c>
-      <c r="E6" s="27">
+      <c r="E6" s="24">
         <v>0.95</v>
       </c>
-      <c r="F6" s="28">
+      <c r="F6" s="25">
         <v>0.95</v>
       </c>
-      <c r="G6" s="29" t="s">
+      <c r="G6" s="26" t="s">
         <v>25</v>
       </c>
       <c r="I6" t="s">
@@ -2307,50 +2326,50 @@
       <c r="A7" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="23">
         <f>B6*(SUM(B3:B4)-B5)</f>
         <v>5.591515427251732</v>
       </c>
-      <c r="C7" s="27">
+      <c r="C7" s="24">
         <f t="shared" ref="C7:F7" si="0">C6*(SUM(C3:C4)-C5)</f>
         <v>4.6931410789473693</v>
       </c>
-      <c r="D7" s="27">
+      <c r="D7" s="24">
         <f t="shared" si="0"/>
         <v>3.7754972929292925</v>
       </c>
-      <c r="E7" s="27">
+      <c r="E7" s="24">
         <f t="shared" si="0"/>
         <v>3.9252004999999994</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="25">
         <f t="shared" si="0"/>
         <v>3.4295551612903217</v>
       </c>
-      <c r="G7" s="29" t="s">
-        <v>72</v>
+      <c r="G7" s="26" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="32">
       <c r="A8" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="23">
         <v>1E-3</v>
       </c>
-      <c r="C8" s="27">
+      <c r="C8" s="24">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="D8" s="27">
+      <c r="D8" s="24">
         <v>0.13400000000000001</v>
       </c>
-      <c r="E8" s="27">
+      <c r="E8" s="24">
         <v>1E-3</v>
       </c>
-      <c r="F8" s="28">
+      <c r="F8" s="25">
         <v>1E-3</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="26" t="s">
         <v>24</v>
       </c>
       <c r="I8" t="s">
@@ -2381,22 +2400,22 @@
       <c r="A9" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="23">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="C9" s="27">
+      <c r="C9" s="24">
         <v>5.0999999999999997E-2</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="24">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="E9" s="27">
+      <c r="E9" s="24">
         <v>0.20599999999999999</v>
       </c>
-      <c r="F9" s="28">
+      <c r="F9" s="25">
         <v>0.13100000000000001</v>
       </c>
-      <c r="G9" s="29" t="s">
+      <c r="G9" s="26" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2404,22 +2423,22 @@
       <c r="A10" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B10" s="26">
+      <c r="B10" s="23">
         <v>0.06</v>
       </c>
-      <c r="C10" s="27">
+      <c r="C10" s="24">
         <v>0.06</v>
       </c>
-      <c r="D10" s="27">
+      <c r="D10" s="24">
         <v>0.06</v>
       </c>
-      <c r="E10" s="27">
+      <c r="E10" s="24">
         <v>0.06</v>
       </c>
-      <c r="F10" s="28">
+      <c r="F10" s="25">
         <v>0.06</v>
       </c>
-      <c r="G10" s="30" t="s">
+      <c r="G10" s="27" t="s">
         <v>67</v>
       </c>
     </row>
@@ -2427,27 +2446,27 @@
       <c r="A11" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="B11" s="26">
+      <c r="B11" s="23">
         <f>$J$24*B7</f>
         <v>0.32852465561674216</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="24">
         <f>$J$24*C7</f>
         <v>0.27574144733778938</v>
       </c>
-      <c r="D11" s="27">
+      <c r="D11" s="24">
         <f>$J$24*D7</f>
         <v>0.22182607990248818</v>
       </c>
-      <c r="E11" s="27">
+      <c r="E11" s="24">
         <f>$J$24*E7</f>
         <v>0.2306217624303282</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="25">
         <f>$J$24*F7</f>
         <v>0.2015005489907592</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="26" t="s">
         <v>59</v>
       </c>
     </row>
@@ -2455,100 +2474,100 @@
       <c r="A12" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B12" s="26">
+      <c r="B12" s="23">
         <v>1.9E-2</v>
       </c>
-      <c r="C12" s="27">
+      <c r="C12" s="24">
         <v>3.6999999999999998E-2</v>
       </c>
-      <c r="D12" s="27">
+      <c r="D12" s="24">
         <v>1.9E-2</v>
       </c>
-      <c r="E12" s="27">
+      <c r="E12" s="24">
         <v>0.17199999999999999</v>
       </c>
-      <c r="F12" s="28">
+      <c r="F12" s="25">
         <v>0.376</v>
       </c>
-      <c r="G12" s="29" t="s">
+      <c r="G12" s="26" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:18">
+    <row r="13" spans="1:18" ht="48">
       <c r="A13" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="26">
-        <v>1.639</v>
-      </c>
-      <c r="C13" s="27">
-        <v>1.4870000000000001</v>
-      </c>
-      <c r="D13" s="27">
-        <v>1.71</v>
-      </c>
-      <c r="E13" s="27">
-        <v>1.6879999999999999</v>
-      </c>
-      <c r="F13" s="28">
+      <c r="B13" s="23">
+        <v>1.8</v>
+      </c>
+      <c r="C13" s="24">
+        <v>1.81</v>
+      </c>
+      <c r="D13" s="24">
+        <v>1.78</v>
+      </c>
+      <c r="E13" s="24">
+        <v>1.7</v>
+      </c>
+      <c r="F13" s="25">
         <v>1.6990000000000001</v>
       </c>
-      <c r="G13" s="29" t="s">
-        <v>71</v>
+      <c r="G13" s="26" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="32">
       <c r="A14" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="26">
+      <c r="B14" s="23">
         <f>2.01+0.385+0.108</f>
         <v>2.5029999999999997</v>
       </c>
-      <c r="C14" s="27">
+      <c r="C14" s="24">
         <f>1.613+0.523+0.1</f>
         <v>2.2360000000000002</v>
       </c>
-      <c r="D14" s="27">
+      <c r="D14" s="24">
         <f>0.579+0.991</f>
         <v>1.5699999999999998</v>
       </c>
-      <c r="E14" s="27">
+      <c r="E14" s="24">
         <v>1.29</v>
       </c>
-      <c r="F14" s="28">
+      <c r="F14" s="25">
         <v>0.85</v>
       </c>
-      <c r="G14" s="29" t="s">
+      <c r="G14" s="26" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="32">
       <c r="A15" s="16" t="s">
-        <v>75</v>
-      </c>
-      <c r="B15" s="26">
+        <v>74</v>
+      </c>
+      <c r="B15" s="23">
         <f>B7-B13-B14-B9-B11+B12+B8</f>
-        <v>1.0479907716349899</v>
-      </c>
-      <c r="C15" s="27">
+        <v>0.8869907716349904</v>
+      </c>
+      <c r="C15" s="24">
         <f>C7-C13-C14-C9-C11+C12+C8</f>
-        <v>0.68439963160957962</v>
-      </c>
-      <c r="D15" s="27">
+        <v>0.36139963160957961</v>
+      </c>
+      <c r="D15" s="24">
         <f>D7-D13-D14-D9-D11+D12+D8</f>
-        <v>0.35267121302680449</v>
-      </c>
-      <c r="E15" s="27">
+        <v>0.28267121302680442</v>
+      </c>
+      <c r="E15" s="28">
         <f>E7-E13-E14-E9-E11+E12+E8</f>
-        <v>0.68357873756967102</v>
-      </c>
-      <c r="F15" s="28">
+        <v>0.67157873756967146</v>
+      </c>
+      <c r="F15" s="29">
         <f>F7-F13-F14-F9-F11+F12+F8</f>
         <v>0.92505461229956243</v>
       </c>
-      <c r="G15" s="29" t="s">
-        <v>73</v>
+      <c r="G15" s="26" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="16" spans="1:18">
@@ -3262,4 +3281,282 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6283D69-CF0D-244D-87FB-05CB70E76780}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="F1" s="33">
+        <v>907</v>
+      </c>
+      <c r="G1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="33"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="33"/>
+      <c r="B3" s="33"/>
+      <c r="C3" s="33"/>
+      <c r="D3" s="33"/>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="33"/>
+      <c r="B4" s="33" t="s">
+        <v>76</v>
+      </c>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="34">
+        <v>1997</v>
+      </c>
+      <c r="B5" s="33">
+        <v>1983.0740000000001</v>
+      </c>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33">
+        <v>1.798648118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="34">
+        <v>1998</v>
+      </c>
+      <c r="B6" s="33">
+        <v>1984.5359999999998</v>
+      </c>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33">
+        <v>1.7999741519999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="34">
+        <v>1999</v>
+      </c>
+      <c r="B7" s="33">
+        <v>1829.3059999999998</v>
+      </c>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33">
+        <v>1.6591805419999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="34">
+        <v>2000</v>
+      </c>
+      <c r="B8" s="33">
+        <v>1854.934</v>
+      </c>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33">
+        <v>1.6824251380000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" s="34">
+        <v>2001</v>
+      </c>
+      <c r="B9" s="33">
+        <v>1830.596</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33">
+        <v>1.660350572</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10" s="34">
+        <v>2002</v>
+      </c>
+      <c r="B10" s="33">
+        <v>1990.8999999999999</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33">
+        <v>1.8057462999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11" s="34">
+        <v>2003</v>
+      </c>
+      <c r="B11" s="33">
+        <v>1844.915</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33">
+        <v>1.6733379050000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12" s="34">
+        <v>2004</v>
+      </c>
+      <c r="B12" s="33">
+        <v>2074.5349999999999</v>
+      </c>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33">
+        <v>1.8816032449999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13" s="34">
+        <v>2005</v>
+      </c>
+      <c r="B13" s="33">
+        <v>1994.34</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33">
+        <v>1.80886638</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14" s="34">
+        <v>2006</v>
+      </c>
+      <c r="B14" s="33">
+        <v>1925.7980000000002</v>
+      </c>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33">
+        <v>1.7466987860000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7">
+      <c r="A15" s="34">
+        <v>2007</v>
+      </c>
+      <c r="B15" s="33">
+        <v>1965.8309999999999</v>
+      </c>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33">
+        <v>1.783008717</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" s="34">
+        <v>2008</v>
+      </c>
+      <c r="B16" s="33">
+        <v>1826.1669999999999</v>
+      </c>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33">
+        <v>1.6563334689999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="34">
+        <v>2009</v>
+      </c>
+      <c r="B17" s="33">
+        <v>1349.125</v>
+      </c>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33">
+        <v>1.223656375</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="34">
+        <v>2010</v>
+      </c>
+      <c r="B18" s="33">
+        <v>1789.4019999999998</v>
+      </c>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33">
+        <v>1.6229876139999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="34">
+        <v>2011</v>
+      </c>
+      <c r="B19" s="33">
+        <v>1846.893</v>
+      </c>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33">
+        <v>1.6751319510000002</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="34">
+        <v>2012</v>
+      </c>
+      <c r="B20" s="33">
+        <v>1870.1990000000001</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33">
+        <v>1.6962704929999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="34">
+        <v>2013</v>
+      </c>
+      <c r="B21" s="33">
+        <v>2020.1399999999999</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33">
+        <v>1.83226698</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="34">
+        <v>2014</v>
+      </c>
+      <c r="B22" s="33">
+        <v>2018.6780000000001</v>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33">
+        <v>1.8309409459999999</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="34">
+        <v>2015</v>
+      </c>
+      <c r="B23" s="33">
+        <v>1834.595</v>
+      </c>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33">
+        <v>1.663977665</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>